<commit_message>
Product Variant and product hierarchy implementation
</commit_message>
<xml_diff>
--- a/imports/Database.xlsx
+++ b/imports/Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Brands en" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="386">
   <si>
     <t xml:space="preserve">Object Name</t>
   </si>
@@ -862,322 +862,331 @@
     <t xml:space="preserve">fridge, cooling</t>
   </si>
   <si>
-    <t xml:space="preserve">Storage Location</t>
+    <t xml:space="preserve">Product Hierarchy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub Categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Rating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Master Image Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Images Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video Poster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity Sold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availablity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selling Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery Charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breadth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimension Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hardware Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wattage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country Of Origin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batteries Required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batteries Included</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motherboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operating System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor Sets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speakers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connectivity Technolgies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronics/Mobiles/BrandX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phones, Accessories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/PRODUCTS/Mobiles/Brand 1/Model 1/images/master.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/PRODUCTS/Laptop/Brand 1/Model 1/video/poster1.png,/PRODUCTS/TV/Brand 1/Model 1/video/poster.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/PRODUCTS/Laptop/Brand 1/Model 1/video/1.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/PRODUCTS/Mobiles/Brand 1/Model 1/video/poster.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of video</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centimeters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB 3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camera 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROM 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screen 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic Sensors Stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speaker2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2G,3G,4G,5G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronics/Tvs/BrandY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TV Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tvs, Accessories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/PRODUCTS/Laptop/Brand 1/Model 1/images/master.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/PRODUCTS/TV/Brand 1/Model 1/images/2.jpeg,/PRODUCTS/Laptop/Brand 1/Model 1/images/2.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laptop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronics/Laptops/BrandXY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laptop Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of the Laptop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laptops, Accessories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/PRODUCTS/TV/Brand 1/Model 1/images/master2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ModelXYZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My Laptop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bluetooth,Edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronics/Mobiles/BrandX/Mobile</t>
   </si>
   <si>
     <t xml:space="preserve">Variant</t>
   </si>
   <si>
-    <t xml:space="preserve">SKU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub Categories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy Rating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Master Image Link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Images Link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Video Link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Video Poster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Video Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Video Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantity Sold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revenue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Availablity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Base Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selling Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delivery Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breadth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dimension Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Size Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hardware Interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voltage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wattage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country Of Origin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Batteries Required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Batteries Included</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motherboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operating System</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sensor Sets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speakers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connectivity Technolgies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronics/Mobiles/BrandX</t>
-  </si>
-  <si>
     <t xml:space="preserve">SKU001</t>
   </si>
   <si>
-    <t xml:space="preserve">Description of Mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phones, Accessories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/PRODUCTS/Mobiles/Brand 1/Model 1/images/master.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/PRODUCTS/Laptop/Brand 1/Model 1/video/poster1.png,/PRODUCTS/TV/Brand 1/Model 1/video/poster.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/PRODUCTS/Laptop/Brand 1/Model 1/video/1.mp4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/PRODUCTS/Mobiles/Brand 1/Model 1/video/poster.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description of video</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centimeters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">My Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB 3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Battery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camera 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROM 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Screen 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic Sensors Stack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speaker2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDD1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2G,3G,4G,5G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronics/Tvs/BrandY</t>
+    <t xml:space="preserve">Red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronics/Tvs/BrandY/TV</t>
   </si>
   <si>
     <t xml:space="preserve">SKU002</t>
   </si>
   <si>
-    <t xml:space="preserve">Description of TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tvs, Accessories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/PRODUCTS/Laptop/Brand 1/Model 1/images/master.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/PRODUCTS/TV/Brand 1/Model 1/images/2.jpeg,/PRODUCTS/Laptop/Brand 1/Model 1/images/2.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model456</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RFID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laptop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronics/Laptops/BrandXY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKU004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laptop1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description of the Laptop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laptops, Accessories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/PRODUCTS/TV/Brand 1/Model 1/images/master2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModelXYZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">My Laptop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bluetooth,Edge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile Red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKU005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Red</t>
+    <t xml:space="preserve">Electronics/Laptops/BrandXY/Laptop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU003</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1196,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1222,6 +1231,17 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1266,7 +1286,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1295,8 +1315,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1319,10 +1343,10 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.13"/>
@@ -1551,13 +1575,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BF5"/>
+  <dimension ref="A1:BF7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AU1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BB1" activeCellId="0" sqref="BB1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.28"/>
@@ -1770,11 +1794,9 @@
         <v>329</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>330</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>328</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>331</v>
@@ -1944,11 +1966,9 @@
         <v>355</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
         <v>356</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>354</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>357</v>
@@ -2104,14 +2124,12 @@
         <v>369</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>23</v>
@@ -2126,7 +2144,7 @@
         <v>242</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>333</v>
@@ -2135,7 +2153,7 @@
         <v>334</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>362</v>
@@ -2147,7 +2165,7 @@
         <v>338</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>340</v>
@@ -2204,13 +2222,13 @@
         <v>342</v>
       </c>
       <c r="AK4" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AL4" s="4" t="n">
         <v>2023</v>
       </c>
       <c r="AM4" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AN4" s="4" t="s">
         <v>366</v>
@@ -2259,24 +2277,21 @@
       <c r="BD4" s="4"/>
       <c r="BE4" s="4"/>
       <c r="BF4" s="4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="46.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="C5" s="8" t="s">
         <v>379</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>328</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>380</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>381</v>
+        <v>328</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>50</v>
@@ -2297,13 +2312,13 @@
         <v>332</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>334</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>362</v>
@@ -2315,7 +2330,7 @@
         <v>338</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>340</v>
@@ -2372,13 +2387,13 @@
         <v>342</v>
       </c>
       <c r="AK5" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AL5" s="4" t="n">
         <v>2023</v>
       </c>
       <c r="AM5" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AN5" s="4" t="s">
         <v>366</v>
@@ -2427,7 +2442,331 @@
       <c r="BD5" s="4"/>
       <c r="BE5" s="4"/>
       <c r="BF5" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="T6" s="4" t="n">
+        <v>150</v>
+      </c>
+      <c r="U6" s="4" t="n">
+        <v>1200</v>
+      </c>
+      <c r="V6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" s="4" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="X6" s="4" t="n">
+        <v>700</v>
+      </c>
+      <c r="Y6" s="4" t="n">
+        <v>900</v>
+      </c>
+      <c r="Z6" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="AA6" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB6" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC6" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AD6" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="AE6" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="AG6" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="AH6" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="AI6" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ6" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="AK6" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="AL6" s="4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="AM6" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="AN6" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="AO6" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="AP6" s="4" t="n">
+        <v>220</v>
+      </c>
+      <c r="AQ6" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="AR6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AS6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="4"/>
+      <c r="AV6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AW6" s="4"/>
+      <c r="AX6" s="4"/>
+      <c r="AY6" s="4"/>
+      <c r="AZ6" s="4"/>
+      <c r="BA6" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="BB6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BC6" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="BD6" s="4"/>
+      <c r="BE6" s="4"/>
+      <c r="BF6" s="4" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="T7" s="4" t="n">
+        <v>120</v>
+      </c>
+      <c r="U7" s="4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="V7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="W7" s="4" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="X7" s="4" t="n">
+        <v>800</v>
+      </c>
+      <c r="Y7" s="4" t="n">
+        <v>1200</v>
+      </c>
+      <c r="Z7" s="4" t="n">
+        <v>70</v>
+      </c>
+      <c r="AA7" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB7" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC7" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AD7" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE7" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AF7" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="AG7" s="4" t="n">
+        <v>45</v>
+      </c>
+      <c r="AH7" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="AI7" s="4" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="AJ7" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="AK7" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="AL7" s="4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="AM7" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="AN7" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="AO7" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="AP7" s="4" t="n">
+        <v>220</v>
+      </c>
+      <c r="AQ7" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="AR7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AS7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU7" s="4"/>
+      <c r="AV7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AW7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AX7" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AY7" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AZ7" s="4"/>
+      <c r="BA7" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="BB7" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BC7" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="BD7" s="4"/>
+      <c r="BE7" s="4"/>
+      <c r="BF7" s="4" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -2449,10 +2788,10 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.01"/>
@@ -2736,10 +3075,10 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.86"/>
@@ -2985,10 +3324,10 @@
   <dimension ref="A1:P1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.29"/>
@@ -3236,10 +3575,10 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.6"/>
@@ -3487,10 +3826,10 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.36"/>
@@ -3619,10 +3958,10 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.13"/>
@@ -3787,11 +4126,11 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23.31"/>
@@ -3967,10 +4306,10 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.03"/>

</xml_diff>